<commit_message>
merge live data feed into quotes workbook
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/Book7.xlsx
+++ b/QuantLibXL/Data2/Book7.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19155" windowHeight="9780" activeTab="6"/>
+    <workbookView xWindow="15330" yWindow="105" windowWidth="14325" windowHeight="8250" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="3M" sheetId="5" r:id="rId1"/>
@@ -2254,7 +2254,7 @@
       </c>
       <c r="I3" s="40" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(H3)</f>
-        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'HKDT3F1_Quote'</v>
+        <v/>
       </c>
       <c r="J3" s="29"/>
     </row>
@@ -2288,7 +2288,7 @@
       </c>
       <c r="I4" s="39" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(H4)</f>
-        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'HKDTOM3F1_Quote'</v>
+        <v/>
       </c>
       <c r="J4" s="29"/>
     </row>
@@ -2319,7 +2319,7 @@
       </c>
       <c r="H5" s="36" t="str">
         <f>_xll.qlFraRateHelper(G5,F5,B5,E5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_1x4F#0002</v>
+        <v>HKD_YC3MRH_1x4F#0001</v>
       </c>
       <c r="I5" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H5)</f>
@@ -2354,7 +2354,7 @@
       </c>
       <c r="H6" s="36" t="str">
         <f>_xll.qlFraRateHelper(G6,F6,B6,E6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_2x5F#0002</v>
+        <v>HKD_YC3MRH_2x5F#0001</v>
       </c>
       <c r="I6" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H6)</f>
@@ -2389,7 +2389,7 @@
       </c>
       <c r="H7" s="36" t="str">
         <f>_xll.qlFraRateHelper(G7,F7,B7,E7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_3x6F#0002</v>
+        <v>HKD_YC3MRH_3x6F#0001</v>
       </c>
       <c r="I7" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H7)</f>
@@ -2424,7 +2424,7 @@
       </c>
       <c r="H8" s="36" t="str">
         <f>_xll.qlFraRateHelper(G8,F8,B8,E8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_4x7F#0002</v>
+        <v>HKD_YC3MRH_4x7F#0001</v>
       </c>
       <c r="I8" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H8)</f>
@@ -2459,7 +2459,7 @@
       </c>
       <c r="H9" s="36" t="str">
         <f>_xll.qlFraRateHelper(G9,F9,B9,E9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_5x8F#0002</v>
+        <v>HKD_YC3MRH_5x8F#0001</v>
       </c>
       <c r="I9" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H9)</f>
@@ -2494,7 +2494,7 @@
       </c>
       <c r="H10" s="36" t="str">
         <f>_xll.qlFraRateHelper(G10,F10,B10,E10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_6x9F#0002</v>
+        <v>HKD_YC3MRH_6x9F#0001</v>
       </c>
       <c r="I10" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H10)</f>
@@ -2529,7 +2529,7 @@
       </c>
       <c r="H11" s="36" t="str">
         <f>_xll.qlFraRateHelper(G11,F11,B11,E11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_7x10F#0002</v>
+        <v>HKD_YC3MRH_7x10F#0001</v>
       </c>
       <c r="I11" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H11)</f>
@@ -2564,7 +2564,7 @@
       </c>
       <c r="H12" s="36" t="str">
         <f>_xll.qlFraRateHelper(G12,F12,B12,E12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_8x11F#0002</v>
+        <v>HKD_YC3MRH_8x11F#0001</v>
       </c>
       <c r="I12" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H12)</f>
@@ -2599,7 +2599,7 @@
       </c>
       <c r="H13" s="31" t="str">
         <f>_xll.qlFraRateHelper(G13,F13,B13,E13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_9x12F#0002</v>
+        <v>HKD_YC3MRH_9x12F#0001</v>
       </c>
       <c r="I13" s="30" t="str">
         <f>_xll.ohRangeRetrieveError(H13)</f>
@@ -2634,14 +2634,14 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="4.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="105.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="3.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="4.28515625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8" style="1"/>
@@ -2719,7 +2719,7 @@
       </c>
       <c r="D8" s="19" t="str">
         <f ca="1">SUBSTITUTE(LEFT(CELL("filename",A1),FIND("[",CELL("filename",A1),1)-1),"\XLS\","\XML\")</f>
-        <v>C:\Users\erik\Documents\repos\quantlib_nando\QuantLibXL\Data2\</v>
+        <v>C:\Projects\quantlib\QuantLibXL\Data2\</v>
       </c>
       <c r="E8" s="16"/>
     </row>
@@ -2962,7 +2962,7 @@
       </c>
       <c r="L4" s="83" t="str">
         <f>_xll.qlIborIndex(K4,FamilyName,J2,S4,Currency,T4,U4,V4,W4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H_Hibor3M#0003</v>
+        <v>HKD_YC3MRH_QM3H_Hibor3M#0002</v>
       </c>
       <c r="M4" s="82" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -3040,7 +3040,7 @@
       </c>
       <c r="L6" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H1Y#0002</v>
+        <v>HKD_YC3MRH_QM3H1Y#0001</v>
       </c>
       <c r="M6" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -3148,7 +3148,7 @@
       </c>
       <c r="L8" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H18M#0002</v>
+        <v>HKD_YC3MRH_QM3H18M#0001</v>
       </c>
       <c r="M8" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -3256,7 +3256,7 @@
       </c>
       <c r="L10" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H2Y#0002</v>
+        <v>HKD_YC3MRH_QM3H2Y#0001</v>
       </c>
       <c r="M10" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -3310,7 +3310,7 @@
       </c>
       <c r="L11" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H3Y#0002</v>
+        <v>HKD_YC3MRH_QM3H3Y#0001</v>
       </c>
       <c r="M11" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -3364,7 +3364,7 @@
       </c>
       <c r="L12" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H4Y#0002</v>
+        <v>HKD_YC3MRH_QM3H4Y#0001</v>
       </c>
       <c r="M12" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -3409,7 +3409,7 @@
       </c>
       <c r="L13" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H5Y#0002</v>
+        <v>HKD_YC3MRH_QM3H5Y#0001</v>
       </c>
       <c r="M13" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -3499,7 +3499,7 @@
       </c>
       <c r="L15" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H7Y#0002</v>
+        <v>HKD_YC3MRH_QM3H7Y#0001</v>
       </c>
       <c r="M15" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -3634,7 +3634,7 @@
       </c>
       <c r="L18" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H10Y#0002</v>
+        <v>HKD_YC3MRH_QM3H10Y#0001</v>
       </c>
       <c r="M18" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -3724,7 +3724,7 @@
       </c>
       <c r="L20" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H12Y#0002</v>
+        <v>HKD_YC3MRH_QM3H12Y#0001</v>
       </c>
       <c r="M20" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -3859,7 +3859,7 @@
       </c>
       <c r="L23" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H15Y#0002</v>
+        <v>HKD_YC3MRH_QM3H15Y#0001</v>
       </c>
       <c r="M23" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="L29" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H21Y#0002</v>
+        <v>HKD_YC3MRH_QM3H21Y#0001</v>
       </c>
       <c r="M29" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -4174,7 +4174,7 @@
       </c>
       <c r="L30" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H22Y#0002</v>
+        <v>HKD_YC3MRH_QM3H22Y#0001</v>
       </c>
       <c r="M30" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -4219,7 +4219,7 @@
       </c>
       <c r="L31" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H23Y#0002</v>
+        <v>HKD_YC3MRH_QM3H23Y#0001</v>
       </c>
       <c r="M31" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -4264,7 +4264,7 @@
       </c>
       <c r="L32" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H24Y#0002</v>
+        <v>HKD_YC3MRH_QM3H24Y#0001</v>
       </c>
       <c r="M32" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -4309,7 +4309,7 @@
       </c>
       <c r="L33" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H25Y#0002</v>
+        <v>HKD_YC3MRH_QM3H25Y#0001</v>
       </c>
       <c r="M33" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -4354,7 +4354,7 @@
       </c>
       <c r="L34" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H26Y#0002</v>
+        <v>HKD_YC3MRH_QM3H26Y#0001</v>
       </c>
       <c r="M34" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -4399,7 +4399,7 @@
       </c>
       <c r="L35" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H27Y#0002</v>
+        <v>HKD_YC3MRH_QM3H27Y#0001</v>
       </c>
       <c r="M35" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -4444,7 +4444,7 @@
       </c>
       <c r="L36" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H28Y#0002</v>
+        <v>HKD_YC3MRH_QM3H28Y#0001</v>
       </c>
       <c r="M36" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -4489,7 +4489,7 @@
       </c>
       <c r="L37" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H29Y#0002</v>
+        <v>HKD_YC3MRH_QM3H29Y#0001</v>
       </c>
       <c r="M37" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -4534,7 +4534,7 @@
       </c>
       <c r="L38" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H30Y#0002</v>
+        <v>HKD_YC3MRH_QM3H30Y#0001</v>
       </c>
       <c r="M38" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -4579,7 +4579,7 @@
       </c>
       <c r="L39" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H35Y#0002</v>
+        <v>HKD_YC3MRH_QM3H35Y#0001</v>
       </c>
       <c r="M39" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L39)</f>
@@ -4624,7 +4624,7 @@
       </c>
       <c r="L40" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H40Y#0002</v>
+        <v>HKD_YC3MRH_QM3H40Y#0001</v>
       </c>
       <c r="M40" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -4669,7 +4669,7 @@
       </c>
       <c r="L41" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H50Y#0002</v>
+        <v>HKD_YC3MRH_QM3H50Y#0001</v>
       </c>
       <c r="M41" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -4714,7 +4714,7 @@
       </c>
       <c r="L42" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H60Y#0002</v>
+        <v>HKD_YC3MRH_QM3H60Y#0001</v>
       </c>
       <c r="M42" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>
@@ -4772,7 +4772,7 @@
       </c>
       <c r="L44" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K44,$J44,$E44&amp;"M",Calendar,$F44,$G44,$H44,$L$4,$I44,B44,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_1S12#0002</v>
+        <v>HKD_YC3MRH_1S12#0001</v>
       </c>
       <c r="M44" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L44)</f>
@@ -4815,7 +4815,7 @@
       </c>
       <c r="L45" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K45,$J45,$E45&amp;"M",Calendar,$F45,$G45,$H45,$L$4,$I45,B45,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_2S12#0002</v>
+        <v>HKD_YC3MRH_2S12#0001</v>
       </c>
       <c r="M45" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L45)</f>
@@ -4860,7 +4860,7 @@
       </c>
       <c r="L46" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K46,$J46,$E46&amp;"M",Calendar,$F46,$G46,$H46,$L$4,$I46,B46,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_3S12#0002</v>
+        <v>HKD_YC3MRH_3S12#0001</v>
       </c>
       <c r="M46" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L46)</f>
@@ -4905,7 +4905,7 @@
       </c>
       <c r="L47" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K47,$J47,$E47&amp;"M",Calendar,$F47,$G47,$H47,$L$4,$I47,B47,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_4S12#0002</v>
+        <v>HKD_YC3MRH_4S12#0001</v>
       </c>
       <c r="M47" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L47)</f>
@@ -4950,7 +4950,7 @@
       </c>
       <c r="L48" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K48,$J48,$E48&amp;"M",Calendar,$F48,$G48,$H48,$L$4,$I48,B48,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_1S24#0002</v>
+        <v>HKD_YC3MRH_1S24#0001</v>
       </c>
       <c r="M48" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L48)</f>
@@ -4995,7 +4995,7 @@
       </c>
       <c r="L49" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K49,$J49,$E49&amp;"M",Calendar,$F49,$G49,$H49,$L$4,$I49,B49,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_2S24#0002</v>
+        <v>HKD_YC3MRH_2S24#0001</v>
       </c>
       <c r="M49" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L49)</f>
@@ -5040,7 +5040,7 @@
       </c>
       <c r="L50" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K50,$J50,$E50&amp;"M",Calendar,$F50,$G50,$H50,$L$4,$I50,B50,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_1S36#0002</v>
+        <v>HKD_YC3MRH_1S36#0001</v>
       </c>
       <c r="M50" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L50)</f>
@@ -5193,7 +5193,7 @@
       </c>
       <c r="D8" s="19" t="str">
         <f ca="1">SUBSTITUTE(LEFT(CELL("filename",A1),FIND("[",CELL("filename",A1),1)-1),"\XLS\","\XML\")</f>
-        <v>C:\Users\erik\Documents\repos\quantlib_nando\QuantLibXL\Data2\</v>
+        <v>C:\Projects\quantlib\QuantLibXL\Data2\</v>
       </c>
       <c r="E8" s="16"/>
     </row>
@@ -6117,11 +6117,11 @@
       </c>
       <c r="L18" s="144">
         <f>_xll.qlRateHelperEarliestDate($E18,Trigger)</f>
-        <v>41626</v>
+        <v>41627</v>
       </c>
       <c r="M18" s="143">
         <f>_xll.qlRateHelperLatestDate($E18,Trigger)</f>
-        <v>41716</v>
+        <v>41717</v>
       </c>
       <c r="P18" s="134" t="e">
         <v>#NUM!</v>
@@ -6207,7 +6207,7 @@
       </c>
       <c r="L20" s="144">
         <f>_xll.qlRateHelperEarliestDate($E20,Trigger)</f>
-        <v>41688</v>
+        <v>41689</v>
       </c>
       <c r="M20" s="143">
         <f>_xll.qlRateHelperLatestDate($E20,Trigger)</f>
@@ -6252,11 +6252,11 @@
       </c>
       <c r="L21" s="144">
         <f>_xll.qlRateHelperEarliestDate($E21,Trigger)</f>
-        <v>41716</v>
+        <v>41717</v>
       </c>
       <c r="M21" s="143">
         <f>_xll.qlRateHelperLatestDate($E21,Trigger)</f>
-        <v>41808</v>
+        <v>41809</v>
       </c>
       <c r="P21" s="134" t="e">
         <v>#NUM!</v>
@@ -6387,11 +6387,11 @@
       </c>
       <c r="L24" s="144">
         <f>_xll.qlRateHelperEarliestDate($E24,Trigger)</f>
-        <v>41808</v>
+        <v>41809</v>
       </c>
       <c r="M24" s="143">
         <f>_xll.qlRateHelperLatestDate($E24,Trigger)</f>
-        <v>41900</v>
+        <v>41901</v>
       </c>
       <c r="P24" s="134" t="e">
         <v>#NUM!</v>
@@ -6432,11 +6432,11 @@
       </c>
       <c r="L25" s="144">
         <f>_xll.qlRateHelperEarliestDate($E25,Trigger)</f>
-        <v>41838</v>
+        <v>41841</v>
       </c>
       <c r="M25" s="143">
         <f>_xll.qlRateHelperLatestDate($E25,Trigger)</f>
-        <v>41932</v>
+        <v>41933</v>
       </c>
       <c r="P25" s="134" t="e">
         <v>#NUM!</v>
@@ -6477,11 +6477,11 @@
       </c>
       <c r="L26" s="144">
         <f>_xll.qlRateHelperEarliestDate($E26,Trigger)</f>
-        <v>41869</v>
+        <v>41870</v>
       </c>
       <c r="M26" s="143">
         <f>_xll.qlRateHelperLatestDate($E26,Trigger)</f>
-        <v>41961</v>
+        <v>41962</v>
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
@@ -9306,11 +9306,11 @@
       </c>
       <c r="L89" s="152">
         <f>_xll.qlRateHelperEarliestDate($E89,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M89" s="151">
         <f>_xll.qlRateHelperLatestDate($E89,Trigger)</f>
-        <v>41961</v>
+        <v>41962</v>
       </c>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.2">
@@ -9348,11 +9348,11 @@
       </c>
       <c r="L90" s="144">
         <f>_xll.qlRateHelperEarliestDate($E90,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M90" s="143">
         <f>_xll.qlRateHelperLatestDate($E90,Trigger)</f>
-        <v>41961</v>
+        <v>41962</v>
       </c>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.2">
@@ -9390,11 +9390,11 @@
       </c>
       <c r="L91" s="144">
         <f>_xll.qlRateHelperEarliestDate($E91,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M91" s="143">
         <f>_xll.qlRateHelperLatestDate($E91,Trigger)</f>
-        <v>41961</v>
+        <v>41962</v>
       </c>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.2">
@@ -9432,11 +9432,11 @@
       </c>
       <c r="L92" s="144">
         <f>_xll.qlRateHelperEarliestDate($E92,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M92" s="143">
         <f>_xll.qlRateHelperLatestDate($E92,Trigger)</f>
-        <v>41961</v>
+        <v>41962</v>
       </c>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.2">
@@ -9474,11 +9474,11 @@
       </c>
       <c r="L93" s="144">
         <f>_xll.qlRateHelperEarliestDate($E93,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M93" s="143">
         <f>_xll.qlRateHelperLatestDate($E93,Trigger)</f>
-        <v>42326</v>
+        <v>42327</v>
       </c>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.2">
@@ -9516,11 +9516,11 @@
       </c>
       <c r="L94" s="144">
         <f>_xll.qlRateHelperEarliestDate($E94,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M94" s="143">
         <f>_xll.qlRateHelperLatestDate($E94,Trigger)</f>
-        <v>42326</v>
+        <v>42327</v>
       </c>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.2">
@@ -9558,11 +9558,11 @@
       </c>
       <c r="L95" s="137">
         <f>_xll.qlRateHelperEarliestDate($E95,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M95" s="136">
         <f>_xll.qlRateHelperLatestDate($E95,Trigger)</f>
-        <v>42692</v>
+        <v>42695</v>
       </c>
     </row>
     <row r="96" spans="2:15" x14ac:dyDescent="0.2">
@@ -9605,11 +9605,11 @@
       </c>
       <c r="L96" s="144">
         <f>_xll.qlRateHelperEarliestDate($E96,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M96" s="143">
         <f>_xll.qlRateHelperLatestDate($E96,Trigger)</f>
-        <v>41961</v>
+        <v>41962</v>
       </c>
       <c r="O96" s="150" t="e">
         <f t="shared" ref="O96:O132" si="9">IF(H96=H133,G96-G133,"--")</f>
@@ -9707,11 +9707,11 @@
       </c>
       <c r="L98" s="144">
         <f>_xll.qlRateHelperEarliestDate($E98,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M98" s="143">
         <f>_xll.qlRateHelperLatestDate($E98,Trigger)</f>
-        <v>42142</v>
+        <v>42143</v>
       </c>
       <c r="O98" s="150" t="e">
         <f t="shared" si="9"/>
@@ -9809,11 +9809,11 @@
       </c>
       <c r="L100" s="144">
         <f>_xll.qlRateHelperEarliestDate($E100,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M100" s="143">
         <f>_xll.qlRateHelperLatestDate($E100,Trigger)</f>
-        <v>42326</v>
+        <v>42327</v>
       </c>
       <c r="O100" s="150" t="e">
         <f t="shared" si="9"/>
@@ -9860,11 +9860,11 @@
       </c>
       <c r="L101" s="144">
         <f>_xll.qlRateHelperEarliestDate($E101,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M101" s="143">
         <f>_xll.qlRateHelperLatestDate($E101,Trigger)</f>
-        <v>42692</v>
+        <v>42695</v>
       </c>
       <c r="O101" s="150" t="e">
         <f t="shared" si="9"/>
@@ -9911,7 +9911,7 @@
       </c>
       <c r="L102" s="144">
         <f>_xll.qlRateHelperEarliestDate($E102,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M102" s="143">
         <f>_xll.qlRateHelperLatestDate($E102,Trigger)</f>
@@ -9962,7 +9962,7 @@
       </c>
       <c r="L103" s="144">
         <f>_xll.qlRateHelperEarliestDate($E103,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M103" s="143">
         <f>_xll.qlRateHelperLatestDate($E103,Trigger)</f>
@@ -10064,11 +10064,11 @@
       </c>
       <c r="L105" s="144">
         <f>_xll.qlRateHelperEarliestDate($E105,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M105" s="143">
         <f>_xll.qlRateHelperLatestDate($E105,Trigger)</f>
-        <v>44153</v>
+        <v>44154</v>
       </c>
       <c r="O105" s="150" t="e">
         <f t="shared" si="9"/>
@@ -10217,7 +10217,7 @@
       </c>
       <c r="L108" s="144">
         <f>_xll.qlRateHelperEarliestDate($E108,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M108" s="143">
         <f>_xll.qlRateHelperLatestDate($E108,Trigger)</f>
@@ -10319,11 +10319,11 @@
       </c>
       <c r="L110" s="144">
         <f>_xll.qlRateHelperEarliestDate($E110,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M110" s="143">
         <f>_xll.qlRateHelperLatestDate($E110,Trigger)</f>
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="O110" s="150" t="e">
         <f t="shared" si="9"/>
@@ -10472,7 +10472,7 @@
       </c>
       <c r="L113" s="144">
         <f>_xll.qlRateHelperEarliestDate($E113,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M113" s="143">
         <f>_xll.qlRateHelperLatestDate($E113,Trigger)</f>
@@ -10778,7 +10778,7 @@
       </c>
       <c r="L119" s="144">
         <f>_xll.qlRateHelperEarliestDate($E119,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M119" s="143">
         <f>_xll.qlRateHelperLatestDate($E119,Trigger)</f>
@@ -10829,7 +10829,7 @@
       </c>
       <c r="L120" s="144">
         <f>_xll.qlRateHelperEarliestDate($E120,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M120" s="143">
         <f>_xll.qlRateHelperLatestDate($E120,Trigger)</f>
@@ -10880,11 +10880,11 @@
       </c>
       <c r="L121" s="144">
         <f>_xll.qlRateHelperEarliestDate($E121,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M121" s="143">
         <f>_xll.qlRateHelperLatestDate($E121,Trigger)</f>
-        <v>49997</v>
+        <v>49998</v>
       </c>
       <c r="O121" s="150" t="e">
         <f t="shared" si="9"/>
@@ -10931,11 +10931,11 @@
       </c>
       <c r="L122" s="144">
         <f>_xll.qlRateHelperEarliestDate($E122,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M122" s="143">
         <f>_xll.qlRateHelperLatestDate($E122,Trigger)</f>
-        <v>50362</v>
+        <v>50363</v>
       </c>
       <c r="O122" s="150" t="e">
         <f t="shared" si="9"/>
@@ -10982,11 +10982,11 @@
       </c>
       <c r="L123" s="144">
         <f>_xll.qlRateHelperEarliestDate($E123,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M123" s="143">
         <f>_xll.qlRateHelperLatestDate($E123,Trigger)</f>
-        <v>50727</v>
+        <v>50728</v>
       </c>
       <c r="O123" s="150" t="e">
         <f t="shared" si="9"/>
@@ -11033,11 +11033,11 @@
       </c>
       <c r="L124" s="144">
         <f>_xll.qlRateHelperEarliestDate($E124,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M124" s="143">
         <f>_xll.qlRateHelperLatestDate($E124,Trigger)</f>
-        <v>51092</v>
+        <v>51095</v>
       </c>
       <c r="O124" s="150" t="e">
         <f t="shared" si="9"/>
@@ -11084,7 +11084,7 @@
       </c>
       <c r="L125" s="144">
         <f>_xll.qlRateHelperEarliestDate($E125,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M125" s="143">
         <f>_xll.qlRateHelperLatestDate($E125,Trigger)</f>
@@ -11135,11 +11135,11 @@
       </c>
       <c r="L126" s="144">
         <f>_xll.qlRateHelperEarliestDate($E126,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M126" s="143">
         <f>_xll.qlRateHelperLatestDate($E126,Trigger)</f>
-        <v>51823</v>
+        <v>51824</v>
       </c>
       <c r="O126" s="150" t="e">
         <f t="shared" si="9"/>
@@ -11186,11 +11186,11 @@
       </c>
       <c r="L127" s="144">
         <f>_xll.qlRateHelperEarliestDate($E127,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M127" s="143">
         <f>_xll.qlRateHelperLatestDate($E127,Trigger)</f>
-        <v>52188</v>
+        <v>52189</v>
       </c>
       <c r="O127" s="150" t="e">
         <f t="shared" si="9"/>
@@ -11237,11 +11237,11 @@
       </c>
       <c r="L128" s="144">
         <f>_xll.qlRateHelperEarliestDate($E128,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M128" s="143">
         <f>_xll.qlRateHelperLatestDate($E128,Trigger)</f>
-        <v>52553</v>
+        <v>52554</v>
       </c>
       <c r="O128" s="150" t="e">
         <f t="shared" si="9"/>
@@ -11288,11 +11288,11 @@
       </c>
       <c r="L129" s="144">
         <f>_xll.qlRateHelperEarliestDate($E129,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M129" s="143">
         <f>_xll.qlRateHelperLatestDate($E129,Trigger)</f>
-        <v>54380</v>
+        <v>54381</v>
       </c>
       <c r="O129" s="150" t="e">
         <f t="shared" si="9"/>
@@ -11339,11 +11339,11 @@
       </c>
       <c r="L130" s="144">
         <f>_xll.qlRateHelperEarliestDate($E130,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M130" s="143">
         <f>_xll.qlRateHelperLatestDate($E130,Trigger)</f>
-        <v>56206</v>
+        <v>56207</v>
       </c>
       <c r="O130" s="150" t="e">
         <f t="shared" si="9"/>
@@ -11390,7 +11390,7 @@
       </c>
       <c r="L131" s="144">
         <f>_xll.qlRateHelperEarliestDate($E131,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M131" s="143">
         <f>_xll.qlRateHelperLatestDate($E131,Trigger)</f>
@@ -11441,7 +11441,7 @@
       </c>
       <c r="L132" s="137">
         <f>_xll.qlRateHelperEarliestDate($E132,Trigger)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="M132" s="136">
         <f>_xll.qlRateHelperLatestDate($E132,Trigger)</f>
@@ -13170,7 +13170,7 @@
   <dimension ref="A1:I126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -13229,14 +13229,14 @@
       </c>
       <c r="G2" s="171">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41626</v>
+        <v>41627</v>
       </c>
       <c r="H2" s="170">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>41716</v>
+        <v>41717</v>
       </c>
       <c r="I2" s="165">
-        <v>0.99865364007964152</v>
+        <v>0.99865364000379186</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -13266,7 +13266,7 @@
         <v>41751</v>
       </c>
       <c r="I3" s="165">
-        <v>0.99826130365752286</v>
+        <v>0.99827251130700834</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -13289,14 +13289,14 @@
       </c>
       <c r="G4" s="171">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41688</v>
+        <v>41689</v>
       </c>
       <c r="H4" s="170">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
         <v>41778</v>
       </c>
       <c r="I4" s="165">
-        <v>0.9979587304392189</v>
+        <v>0.9979699290571088</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -13319,14 +13319,14 @@
       </c>
       <c r="G5" s="171">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41716</v>
+        <v>41717</v>
       </c>
       <c r="H5" s="170">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>41808</v>
+        <v>41809</v>
       </c>
       <c r="I5" s="165">
-        <v>0.99757243554392094</v>
+        <v>0.99757243546815444</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -13357,7 +13357,7 @@
         <v>41842</v>
       </c>
       <c r="I6" s="165">
-        <v>0.99716742465262953</v>
+        <v>0.99717862002060087</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -13389,7 +13389,7 @@
         <v>41870</v>
       </c>
       <c r="I7" s="165">
-        <v>0.99682808160116487</v>
+        <v>0.99683926753185581</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -13406,14 +13406,14 @@
       </c>
       <c r="G8" s="171">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41808</v>
+        <v>41809</v>
       </c>
       <c r="H8" s="170">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>41900</v>
+        <v>41901</v>
       </c>
       <c r="I8" s="165">
-        <v>0.99639205219210403</v>
+        <v>0.99639205211643067</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -13430,14 +13430,14 @@
       </c>
       <c r="G9" s="171">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>41838</v>
+        <v>41841</v>
       </c>
       <c r="H9" s="170">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>41932</v>
+        <v>41933</v>
       </c>
       <c r="I9" s="165">
-        <v>0.99598399997198916</v>
+        <v>0.99598562164313242</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -13454,14 +13454,14 @@
       </c>
       <c r="G10" s="171">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="H10" s="170">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>41961</v>
+        <v>41962</v>
       </c>
       <c r="I10" s="165">
-        <v>0.99561169152995321</v>
+        <v>0.99561169515438841</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -13478,14 +13478,14 @@
       </c>
       <c r="G11" s="171">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="H11" s="170">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>42142</v>
+        <v>42143</v>
       </c>
       <c r="I11" s="165">
-        <v>0.99284777325285223</v>
+        <v>0.99284777808043889</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -13503,14 +13503,14 @@
       </c>
       <c r="G12" s="171">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="H12" s="170">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>42326</v>
+        <v>42327</v>
       </c>
       <c r="I12" s="165">
-        <v>0.98925811737838731</v>
+        <v>0.98925812337415742</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -13528,14 +13528,14 @@
       </c>
       <c r="G13" s="171">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="H13" s="170">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>42692</v>
+        <v>42695</v>
       </c>
       <c r="I13" s="165">
-        <v>0.9770996947370767</v>
+        <v>0.97705845058217056</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -13552,14 +13552,14 @@
       </c>
       <c r="G14" s="171">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="H14" s="170">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
         <v>43059</v>
       </c>
       <c r="I14" s="165">
-        <v>0.95700518745974861</v>
+        <v>0.95703325949529394</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -13576,14 +13576,14 @@
       </c>
       <c r="G15" s="171">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="H15" s="170">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
         <v>43423</v>
       </c>
       <c r="I15" s="165">
-        <v>0.93114705564664457</v>
+        <v>0.93118294061173668</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -13600,14 +13600,14 @@
       </c>
       <c r="G16" s="171">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="H16" s="170">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>44153</v>
+        <v>44154</v>
       </c>
       <c r="I16" s="165">
-        <v>0.86979090364821499</v>
+        <v>0.869791904909194</v>
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.2">
@@ -13624,14 +13624,14 @@
       </c>
       <c r="G17" s="171">
         <f>_xll.qlRateHelperEarliestDate($D17)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="H17" s="170">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
         <v>45250</v>
       </c>
       <c r="I17" s="165">
-        <v>0.77614369384905335</v>
+        <v>0.77619760049330866</v>
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.2">
@@ -13648,14 +13648,14 @@
       </c>
       <c r="G18" s="171">
         <f>_xll.qlRateHelperEarliestDate($D18)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="H18" s="170">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="I18" s="165">
-        <v>0.72266647460738664</v>
+        <v>0.72266935831338064</v>
       </c>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.2">
@@ -13672,14 +13672,14 @@
       </c>
       <c r="G19" s="171">
         <f>_xll.qlRateHelperEarliestDate($D19)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="H19" s="170">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
         <v>47077</v>
       </c>
       <c r="I19" s="165">
-        <v>0.65492494470752005</v>
+        <v>0.65497637364458239</v>
       </c>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.2">
@@ -16270,7 +16270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17254,7 +17254,7 @@
       <c r="B27" s="98"/>
       <c r="C27" s="102">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41596</v>
+        <v>41597</v>
       </c>
       <c r="D27" s="101">
         <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
@@ -17299,7 +17299,7 @@
       </c>
       <c r="D28" s="99">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>0.65492494470752005</v>
+        <v>0.65497637364458239</v>
       </c>
       <c r="E28" s="95"/>
       <c r="F28" s="94"/>

</xml_diff>